<commit_message>
fixed lifefinance crash with name
</commit_message>
<xml_diff>
--- a/resources/input/input hrefs.xlsx
+++ b/resources/input/input hrefs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\traiding\v2\resources\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\traiding\sites_scraper\resources\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7005CE31-ACA0-4FDC-BE76-822CD5A6B505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -27,13 +28,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>https://copy6.forex4you.org/ru/leaders#/8120331/trades</t>
+    <t>https://my.litefinance.org/ru/traders/trades-history?id=2187036</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -344,16 +345,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="103.375" customWidth="1"/>
+    <col min="1" max="1" width="103.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -368,7 +369,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>